<commit_message>
update schematic   -> use LTC2950 : Push Button On/Off Controller   -> re-assign pin   -> change EEPROM from SPI to I2C interface   -> SD-Card move from SPI2 to SPI1
</commit_message>
<xml_diff>
--- a/doc/MAX1676-Low Battery Detection Register Calculator.xlsx
+++ b/doc/MAX1676-Low Battery Detection Register Calculator.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>R3</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,6 +47,26 @@
   </si>
   <si>
     <t>270K</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LTC2950 Capacitor vs Delay time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T(ms)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C(uF)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coef</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -54,6 +74,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="0_ "/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -93,8 +116,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -377,15 +409,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F14"/>
+  <dimension ref="B1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="12" max="12" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -398,8 +439,20 @@
       <c r="F2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -416,8 +469,18 @@
       <c r="F3">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I3" s="2">
+        <v>1.56E-4</v>
+      </c>
+      <c r="J3">
+        <v>500</v>
+      </c>
+      <c r="L3">
+        <f>I3*(J3-1)</f>
+        <v>7.7843999999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C4">
         <f t="shared" ref="C4:C8" si="0">D4*((E4/F4)-1)</f>
         <v>332307.69230769231</v>
@@ -431,8 +494,18 @@
       <c r="F4">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I4" s="2">
+        <v>1.56E-4</v>
+      </c>
+      <c r="J4">
+        <v>1000</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L8" si="1">I4*(J4-1)</f>
+        <v>0.15584400000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C5">
         <f t="shared" si="0"/>
         <v>350769.23076923081</v>
@@ -446,8 +519,19 @@
       <c r="F5">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I5" s="2">
+        <v>1.56E-4</v>
+      </c>
+      <c r="J5">
+        <v>1500</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>0.233844</v>
+      </c>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C6">
         <f t="shared" si="0"/>
         <v>369230.76923076919</v>
@@ -461,8 +545,18 @@
       <c r="F6">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I6" s="2">
+        <v>1.56E-4</v>
+      </c>
+      <c r="J6">
+        <v>2000</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>0.31184400000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C7">
         <f t="shared" si="0"/>
         <v>387692.30769230769</v>
@@ -476,8 +570,18 @@
       <c r="F7">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I7" s="2">
+        <v>1.56E-4</v>
+      </c>
+      <c r="J7">
+        <v>2500</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>0.38984399999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C8">
         <f t="shared" si="0"/>
         <v>406153.84615384607</v>
@@ -491,13 +595,23 @@
       <c r="F8">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I8" s="2">
+        <v>1.56E-4</v>
+      </c>
+      <c r="J8">
+        <v>3000</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>0.46784399999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:C14" si="1">D9*((E9/F9)-1)</f>
+        <f t="shared" ref="C9:C14" si="2">D9*((E9/F9)-1)</f>
         <v>261538.4615384615</v>
       </c>
       <c r="D9">
@@ -510,9 +624,9 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>276923.07692307694</v>
       </c>
       <c r="D10">
@@ -524,10 +638,19 @@
       <c r="F10">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>292307.69230769231</v>
       </c>
       <c r="D11">
@@ -539,10 +662,20 @@
       <c r="F11">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I11" s="2">
+        <v>1.56E-4</v>
+      </c>
+      <c r="J11">
+        <v>0.01</v>
+      </c>
+      <c r="L11" s="3">
+        <f>J11/I11+1</f>
+        <v>65.102564102564102</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>307692.30769230769</v>
       </c>
       <c r="D12">
@@ -554,10 +687,20 @@
       <c r="F12">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I12" s="2">
+        <v>1.56E-4</v>
+      </c>
+      <c r="J12">
+        <v>0.1</v>
+      </c>
+      <c r="L12" s="3">
+        <f t="shared" ref="L12:L14" si="3">J12/I12+1</f>
+        <v>642.02564102564111</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>323076.92307692306</v>
       </c>
       <c r="D13">
@@ -569,10 +712,20 @@
       <c r="F13">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I13" s="2">
+        <v>1.56E-4</v>
+      </c>
+      <c r="J13">
+        <v>0.3</v>
+      </c>
+      <c r="L13" s="3">
+        <f t="shared" si="3"/>
+        <v>1924.0769230769231</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>338461.53846153844</v>
       </c>
       <c r="D14">
@@ -583,6 +736,28 @@
       </c>
       <c r="F14">
         <v>1.3</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1.56E-4</v>
+      </c>
+      <c r="J14">
+        <v>0.47</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" si="3"/>
+        <v>3013.8205128205127</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I15" s="2">
+        <v>1.56E-4</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3">
+        <f t="shared" ref="L15" si="4">J15/I15+1</f>
+        <v>6411.2564102564102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>